<commit_message>
Monday lec1 and lec2 btns link working
</commit_message>
<xml_diff>
--- a/My_Folder/sample3.xlsx
+++ b/My_Folder/sample3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abhis\Desktop\SDP_Works\Time_Table_Linker_Project\My_Folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B54B700-DDCE-48CC-9769-F8A25CAF3305}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09E067A8-9DC8-48D9-8961-B196D80D63D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="45">
   <si>
     <t>Time</t>
   </si>
@@ -160,9 +160,6 @@
   </si>
   <si>
     <t>AXS</t>
-  </si>
-  <si>
-    <t>CAOS LL</t>
   </si>
 </sst>
 </file>
@@ -513,7 +510,7 @@
   <dimension ref="A1:W11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -561,7 +558,7 @@
         <v>11</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1" t="s">
@@ -612,7 +609,7 @@
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="Q3" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="R3" s="1" t="s">
         <v>34</v>
@@ -647,7 +644,7 @@
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="Q4" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="R4" s="1" t="s">
         <v>35</v>

</xml_diff>

<commit_message>
Pushing before removing the buttons-link
</commit_message>
<xml_diff>
--- a/My_Folder/sample3.xlsx
+++ b/My_Folder/sample3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abhis\Desktop\SDP_Works\Time_Table_Linker_Project\My_Folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09E067A8-9DC8-48D9-8961-B196D80D63D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70EED688-AA89-4477-B75F-384A548FE281}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12360" tabRatio="639" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="38">
   <si>
     <t>Time</t>
   </si>
@@ -84,36 +84,15 @@
     <t>Wednesday</t>
   </si>
   <si>
-    <t>DS</t>
-  </si>
-  <si>
     <t>Thursday</t>
   </si>
   <si>
-    <t>DDB DCAN TUT</t>
-  </si>
-  <si>
-    <t>QRS</t>
-  </si>
-  <si>
     <t>SDP</t>
   </si>
   <si>
-    <t>VDP</t>
-  </si>
-  <si>
     <t>Friday</t>
   </si>
   <si>
-    <t>EFG</t>
-  </si>
-  <si>
-    <t>ABC</t>
-  </si>
-  <si>
-    <t>KLM</t>
-  </si>
-  <si>
     <t>Saturday</t>
   </si>
   <si>
@@ -159,7 +138,7 @@
     <t>VLK</t>
   </si>
   <si>
-    <t>AXS</t>
+    <t>https://meet.google.com/khj-syqw-kvz</t>
   </si>
 </sst>
 </file>
@@ -183,7 +162,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -206,26 +185,14 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -507,13 +474,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W11"/>
+  <dimension ref="A1:W10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
@@ -547,7 +518,7 @@
         <v>9</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.3">
@@ -555,15 +526,13 @@
         <v>10</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D2" s="1"/>
-      <c r="E2" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="E2" s="1"/>
       <c r="F2" s="1" t="s">
         <v>14</v>
       </c>
@@ -577,7 +546,7 @@
         <v>11</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
@@ -590,7 +559,7 @@
         <v>16</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>12</v>
@@ -600,7 +569,7 @@
         <v>13</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1" t="s">
@@ -612,7 +581,7 @@
         <v>12</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
@@ -625,29 +594,35 @@
         <v>18</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="1"/>
+      <c r="D4" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="E4" s="1" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="1"/>
+      <c r="G4" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="H4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I4" s="1"/>
+        <v>15</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="J4" s="1"/>
       <c r="Q4" s="1" t="s">
         <v>13</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="S4" s="1"/>
       <c r="T4" s="1"/>
@@ -657,34 +632,30 @@
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="D5" s="1"/>
-      <c r="E5" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>23</v>
-      </c>
+      <c r="E5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="3"/>
       <c r="G5" s="1"/>
-      <c r="H5" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="Q5" s="1" t="s">
         <v>14</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
@@ -694,36 +665,32 @@
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>24</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="D6" s="1"/>
       <c r="E6" s="1" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>28</v>
-      </c>
+      <c r="H6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
       <c r="Q6" s="1" t="s">
         <v>15</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="S6" s="1"/>
       <c r="T6" s="1"/>
@@ -733,32 +700,32 @@
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="Q7" s="1" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="S7" s="1"/>
       <c r="T7" s="1"/>
@@ -768,10 +735,10 @@
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.3">
       <c r="Q8" s="1" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="R8" s="1" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="S8" s="1"/>
       <c r="T8" s="1"/>
@@ -781,10 +748,10 @@
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.3">
       <c r="Q9" s="1" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="R9" s="1" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="S9" s="1"/>
       <c r="T9" s="1"/>
@@ -794,10 +761,10 @@
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.3">
       <c r="Q10" s="1" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="R10" s="1" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="S10" s="1"/>
       <c r="T10" s="1"/>
@@ -805,19 +772,6 @@
       <c r="V10" s="1"/>
       <c r="W10" s="1"/>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="Q11" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="R11" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="S11" s="1"/>
-      <c r="T11" s="1"/>
-      <c r="U11" s="1"/>
-      <c r="V11" s="1"/>
-      <c r="W11" s="1"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Before removing the confusing buttons of saturday
</commit_message>
<xml_diff>
--- a/My_Folder/sample3.xlsx
+++ b/My_Folder/sample3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abhis\Desktop\SDP_Works\Time_Table_Linker_Project\My_Folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70EED688-AA89-4477-B75F-384A548FE281}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00421C08-D76D-4974-9575-C2B374498CD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12360" tabRatio="639" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="40">
   <si>
     <t>Time</t>
   </si>
@@ -139,6 +139,12 @@
   </si>
   <si>
     <t>https://meet.google.com/khj-syqw-kvz</t>
+  </si>
+  <si>
+    <t>POL</t>
+  </si>
+  <si>
+    <t>https://meet.google.com/abc?pli=1&amp;authuser=1</t>
   </si>
 </sst>
 </file>
@@ -154,15 +160,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -185,15 +197,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -474,10 +499,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W10"/>
+  <dimension ref="A1:W11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -526,22 +551,32 @@
         <v>10</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
+      <c r="D2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="F2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="1"/>
+      <c r="G2" s="4" t="s">
+        <v>38</v>
+      </c>
       <c r="H2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
+      <c r="I2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="Q2" s="1" t="s">
         <v>11</v>
       </c>
@@ -617,7 +652,7 @@
       <c r="I4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J4" s="1"/>
+      <c r="J4" s="5"/>
       <c r="Q4" s="1" t="s">
         <v>13</v>
       </c>
@@ -645,9 +680,13 @@
         <v>12</v>
       </c>
       <c r="F5" s="3"/>
-      <c r="G5" s="1"/>
+      <c r="G5" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
+      <c r="I5" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="J5" s="1" t="s">
         <v>34</v>
       </c>
@@ -680,12 +719,18 @@
       <c r="F6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G6" s="1"/>
+      <c r="G6" s="4" t="s">
+        <v>38</v>
+      </c>
       <c r="H6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
+      <c r="I6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="Q6" s="1" t="s">
         <v>15</v>
       </c>
@@ -709,7 +754,7 @@
         <v>24</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1" t="s">
@@ -718,9 +763,15 @@
       <c r="G7" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
+      <c r="H7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="Q7" s="1" t="s">
         <v>31</v>
       </c>
@@ -772,7 +823,16 @@
       <c r="V10" s="1"/>
       <c r="W10" s="1"/>
     </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="Q11" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="R11" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added day recognizer fuction | Before removing saturday buttons
</commit_message>
<xml_diff>
--- a/My_Folder/sample3.xlsx
+++ b/My_Folder/sample3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abhis\Desktop\SDP_Works\Time_Table_Linker_Project\My_Folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00421C08-D76D-4974-9575-C2B374498CD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B51CB030-9304-41A9-A5CE-E88DEA944396}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12360" tabRatio="639" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -160,7 +160,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -170,6 +170,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -212,13 +218,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -502,7 +509,7 @@
   <dimension ref="A1:W11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -744,32 +751,32 @@
       <c r="W6" s="1"/>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1" t="s">
+      <c r="E7" s="6"/>
+      <c r="F7" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="G7" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H7" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="I7" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="J7" s="6" t="s">
         <v>15</v>
       </c>
       <c r="Q7" s="1" t="s">

</xml_diff>